<commit_message>
Deploying to gh-pages from @ aehrc/genclipr-fhir-ig@d06eb29f8e4ceaba7d7f0a1e658d0bbd00181724 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-LaboratoryFinding.xlsx
+++ b/StructureDefinition-LaboratoryFinding.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2545" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2544" uniqueCount="468">
   <si>
     <t>Path</t>
   </si>
@@ -834,10 +834,7 @@
     <t>For some results, particularly numeric results, an interpretation is necessary to fully understand the significance of a result.</t>
   </si>
   <si>
-    <t>Codes identifying interpretations of observations.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/observation-interpretation</t>
+    <t>http://aehrc.github.io/genclipr-fhir-ig/ValueSet/TestInterpretationValues</t>
   </si>
   <si>
     <t>&lt; 260245000 |Findings values|</t>
@@ -1313,6 +1310,12 @@
   </si>
   <si>
     <t>Observation.component.interpretation</t>
+  </si>
+  <si>
+    <t>Codes identifying interpretations of observations.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/observation-interpretation</t>
   </si>
   <si>
     <t>Observation.component.referenceRange</t>
@@ -4516,7 +4519,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" hidden="true">
+    <row r="25">
       <c r="A25" t="s" s="2">
         <v>253</v>
       </c>
@@ -4532,7 +4535,7 @@
         <v>43</v>
       </c>
       <c r="G25" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H25" t="s" s="2">
         <v>45</v>
@@ -4578,13 +4581,11 @@
         <v>45</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="X25" t="s" s="2">
+        <v>144</v>
+      </c>
+      <c r="X25" s="2"/>
+      <c r="Y25" t="s" s="2">
         <v>259</v>
-      </c>
-      <c r="Y25" t="s" s="2">
-        <v>260</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>45</v>
@@ -4620,24 +4621,24 @@
         <v>45</v>
       </c>
       <c r="AK25" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="AL25" t="s" s="2">
         <v>261</v>
       </c>
-      <c r="AL25" t="s" s="2">
+      <c r="AM25" t="s" s="2">
         <v>262</v>
       </c>
-      <c r="AM25" t="s" s="2">
+      <c r="AN25" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO25" t="s" s="2">
         <v>263</v>
-      </c>
-      <c r="AN25" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO25" t="s" s="2">
-        <v>264</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4660,19 +4661,19 @@
         <v>45</v>
       </c>
       <c r="J26" t="s" s="2">
+        <v>265</v>
+      </c>
+      <c r="K26" t="s" s="2">
         <v>266</v>
       </c>
-      <c r="K26" t="s" s="2">
+      <c r="L26" t="s" s="2">
         <v>267</v>
       </c>
-      <c r="L26" t="s" s="2">
+      <c r="M26" t="s" s="2">
         <v>268</v>
       </c>
-      <c r="M26" t="s" s="2">
+      <c r="N26" t="s" s="2">
         <v>269</v>
-      </c>
-      <c r="N26" t="s" s="2">
-        <v>270</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>45</v>
@@ -4721,7 +4722,7 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -4742,10 +4743,10 @@
         <v>45</v>
       </c>
       <c r="AL26" t="s" s="2">
+        <v>270</v>
+      </c>
+      <c r="AM26" t="s" s="2">
         <v>271</v>
-      </c>
-      <c r="AM26" t="s" s="2">
-        <v>272</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>45</v>
@@ -4756,7 +4757,7 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4782,13 +4783,13 @@
         <v>153</v>
       </c>
       <c r="K27" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="L27" t="s" s="2">
         <v>274</v>
       </c>
-      <c r="L27" t="s" s="2">
+      <c r="M27" t="s" s="2">
         <v>275</v>
-      </c>
-      <c r="M27" t="s" s="2">
-        <v>276</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
@@ -4814,14 +4815,14 @@
         <v>45</v>
       </c>
       <c r="W27" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="X27" t="s" s="2">
         <v>277</v>
       </c>
-      <c r="X27" t="s" s="2">
+      <c r="Y27" t="s" s="2">
         <v>278</v>
       </c>
-      <c r="Y27" t="s" s="2">
-        <v>279</v>
-      </c>
       <c r="Z27" t="s" s="2">
         <v>45</v>
       </c>
@@ -4838,7 +4839,7 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
@@ -4856,24 +4857,24 @@
         <v>45</v>
       </c>
       <c r="AK27" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="AL27" t="s" s="2">
         <v>280</v>
       </c>
-      <c r="AL27" t="s" s="2">
+      <c r="AM27" t="s" s="2">
         <v>281</v>
       </c>
-      <c r="AM27" t="s" s="2">
+      <c r="AN27" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO27" t="s" s="2">
         <v>282</v>
-      </c>
-      <c r="AN27" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO27" t="s" s="2">
-        <v>283</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4899,16 +4900,16 @@
         <v>153</v>
       </c>
       <c r="K28" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="L28" t="s" s="2">
         <v>285</v>
       </c>
-      <c r="L28" t="s" s="2">
+      <c r="M28" t="s" s="2">
         <v>286</v>
       </c>
-      <c r="M28" t="s" s="2">
+      <c r="N28" t="s" s="2">
         <v>287</v>
-      </c>
-      <c r="N28" t="s" s="2">
-        <v>288</v>
       </c>
       <c r="O28" t="s" s="2">
         <v>45</v>
@@ -4933,14 +4934,14 @@
         <v>45</v>
       </c>
       <c r="W28" t="s" s="2">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="X28" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="Y28" t="s" s="2">
         <v>289</v>
       </c>
-      <c r="Y28" t="s" s="2">
-        <v>290</v>
-      </c>
       <c r="Z28" t="s" s="2">
         <v>45</v>
       </c>
@@ -4957,7 +4958,7 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -4978,10 +4979,10 @@
         <v>45</v>
       </c>
       <c r="AL28" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="AM28" t="s" s="2">
         <v>291</v>
-      </c>
-      <c r="AM28" t="s" s="2">
-        <v>292</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>45</v>
@@ -4992,7 +4993,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -5015,16 +5016,16 @@
         <v>45</v>
       </c>
       <c r="J29" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="K29" t="s" s="2">
         <v>294</v>
       </c>
-      <c r="K29" t="s" s="2">
+      <c r="L29" t="s" s="2">
         <v>295</v>
       </c>
-      <c r="L29" t="s" s="2">
+      <c r="M29" t="s" s="2">
         <v>296</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>297</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
@@ -5074,7 +5075,7 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
@@ -5092,24 +5093,24 @@
         <v>45</v>
       </c>
       <c r="AK29" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="AL29" t="s" s="2">
         <v>298</v>
       </c>
-      <c r="AL29" t="s" s="2">
+      <c r="AM29" t="s" s="2">
         <v>299</v>
       </c>
-      <c r="AM29" t="s" s="2">
+      <c r="AN29" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO29" t="s" s="2">
         <v>300</v>
-      </c>
-      <c r="AN29" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO29" t="s" s="2">
-        <v>301</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -5132,16 +5133,16 @@
         <v>45</v>
       </c>
       <c r="J30" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="K30" t="s" s="2">
         <v>303</v>
       </c>
-      <c r="K30" t="s" s="2">
+      <c r="L30" t="s" s="2">
         <v>304</v>
       </c>
-      <c r="L30" t="s" s="2">
+      <c r="M30" t="s" s="2">
         <v>305</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>306</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -5191,7 +5192,7 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -5209,24 +5210,24 @@
         <v>45</v>
       </c>
       <c r="AK30" t="s" s="2">
+        <v>306</v>
+      </c>
+      <c r="AL30" t="s" s="2">
         <v>307</v>
       </c>
-      <c r="AL30" t="s" s="2">
+      <c r="AM30" t="s" s="2">
         <v>308</v>
       </c>
-      <c r="AM30" t="s" s="2">
+      <c r="AN30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO30" t="s" s="2">
         <v>309</v>
-      </c>
-      <c r="AN30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO30" t="s" s="2">
-        <v>310</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5249,19 +5250,19 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="K31" t="s" s="2">
         <v>312</v>
       </c>
-      <c r="K31" t="s" s="2">
+      <c r="L31" t="s" s="2">
         <v>313</v>
       </c>
-      <c r="L31" t="s" s="2">
+      <c r="M31" t="s" s="2">
         <v>314</v>
       </c>
-      <c r="M31" t="s" s="2">
+      <c r="N31" t="s" s="2">
         <v>315</v>
-      </c>
-      <c r="N31" t="s" s="2">
-        <v>316</v>
       </c>
       <c r="O31" t="s" s="2">
         <v>45</v>
@@ -5310,7 +5311,7 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -5322,19 +5323,19 @@
         <v>45</v>
       </c>
       <c r="AI31" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="AJ31" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK31" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL31" t="s" s="2">
         <v>317</v>
       </c>
-      <c r="AJ31" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK31" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL31" t="s" s="2">
+      <c r="AM31" t="s" s="2">
         <v>318</v>
-      </c>
-      <c r="AM31" t="s" s="2">
-        <v>319</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
@@ -5345,7 +5346,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5371,10 +5372,10 @@
         <v>57</v>
       </c>
       <c r="K32" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="L32" t="s" s="2">
         <v>321</v>
-      </c>
-      <c r="L32" t="s" s="2">
-        <v>322</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -5425,7 +5426,7 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -5449,7 +5450,7 @@
         <v>45</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
@@ -5460,7 +5461,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5489,7 +5490,7 @@
         <v>102</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="M33" t="s" s="2">
         <v>104</v>
@@ -5542,7 +5543,7 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
@@ -5566,7 +5567,7 @@
         <v>45</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
@@ -5577,11 +5578,11 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
@@ -5603,10 +5604,10 @@
         <v>101</v>
       </c>
       <c r="K34" t="s" s="2">
+        <v>329</v>
+      </c>
+      <c r="L34" t="s" s="2">
         <v>330</v>
-      </c>
-      <c r="L34" t="s" s="2">
-        <v>331</v>
       </c>
       <c r="M34" t="s" s="2">
         <v>104</v>
@@ -5661,7 +5662,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5696,7 +5697,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5719,13 +5720,13 @@
         <v>45</v>
       </c>
       <c r="J35" t="s" s="2">
+        <v>333</v>
+      </c>
+      <c r="K35" t="s" s="2">
         <v>334</v>
       </c>
-      <c r="K35" t="s" s="2">
+      <c r="L35" t="s" s="2">
         <v>335</v>
-      </c>
-      <c r="L35" t="s" s="2">
-        <v>336</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5776,7 +5777,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5785,7 +5786,7 @@
         <v>55</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>67</v>
@@ -5797,10 +5798,10 @@
         <v>45</v>
       </c>
       <c r="AL35" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="AM35" t="s" s="2">
         <v>338</v>
-      </c>
-      <c r="AM35" t="s" s="2">
-        <v>339</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -5811,7 +5812,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5834,13 +5835,13 @@
         <v>45</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="K36" t="s" s="2">
+        <v>340</v>
+      </c>
+      <c r="L36" t="s" s="2">
         <v>341</v>
-      </c>
-      <c r="L36" t="s" s="2">
-        <v>342</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5891,7 +5892,7 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
@@ -5900,7 +5901,7 @@
         <v>55</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AI36" t="s" s="2">
         <v>67</v>
@@ -5912,10 +5913,10 @@
         <v>45</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>45</v>
@@ -5926,7 +5927,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5952,16 +5953,16 @@
         <v>153</v>
       </c>
       <c r="K37" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="L37" t="s" s="2">
         <v>345</v>
       </c>
-      <c r="L37" t="s" s="2">
+      <c r="M37" t="s" s="2">
         <v>346</v>
       </c>
-      <c r="M37" t="s" s="2">
+      <c r="N37" t="s" s="2">
         <v>347</v>
-      </c>
-      <c r="N37" t="s" s="2">
-        <v>348</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>45</v>
@@ -5989,11 +5990,11 @@
         <v>79</v>
       </c>
       <c r="X37" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="Y37" t="s" s="2">
         <v>349</v>
       </c>
-      <c r="Y37" t="s" s="2">
-        <v>350</v>
-      </c>
       <c r="Z37" t="s" s="2">
         <v>45</v>
       </c>
@@ -6010,7 +6011,7 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
@@ -6028,13 +6029,13 @@
         <v>45</v>
       </c>
       <c r="AK37" t="s" s="2">
+        <v>350</v>
+      </c>
+      <c r="AL37" t="s" s="2">
         <v>351</v>
       </c>
-      <c r="AL37" t="s" s="2">
-        <v>352</v>
-      </c>
       <c r="AM37" t="s" s="2">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>45</v>
@@ -6045,7 +6046,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -6071,16 +6072,16 @@
         <v>153</v>
       </c>
       <c r="K38" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="L38" t="s" s="2">
         <v>354</v>
       </c>
-      <c r="L38" t="s" s="2">
+      <c r="M38" t="s" s="2">
         <v>355</v>
       </c>
-      <c r="M38" t="s" s="2">
+      <c r="N38" t="s" s="2">
         <v>356</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>357</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>45</v>
@@ -6105,14 +6106,14 @@
         <v>45</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="X38" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="Y38" t="s" s="2">
         <v>358</v>
       </c>
-      <c r="Y38" t="s" s="2">
-        <v>359</v>
-      </c>
       <c r="Z38" t="s" s="2">
         <v>45</v>
       </c>
@@ -6129,7 +6130,7 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
@@ -6147,13 +6148,13 @@
         <v>45</v>
       </c>
       <c r="AK38" t="s" s="2">
+        <v>350</v>
+      </c>
+      <c r="AL38" t="s" s="2">
         <v>351</v>
       </c>
-      <c r="AL38" t="s" s="2">
-        <v>352</v>
-      </c>
       <c r="AM38" t="s" s="2">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
@@ -6164,7 +6165,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6187,17 +6188,17 @@
         <v>45</v>
       </c>
       <c r="J39" t="s" s="2">
+        <v>360</v>
+      </c>
+      <c r="K39" t="s" s="2">
         <v>361</v>
       </c>
-      <c r="K39" t="s" s="2">
+      <c r="L39" t="s" s="2">
         <v>362</v>
-      </c>
-      <c r="L39" t="s" s="2">
-        <v>363</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" t="s" s="2">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>45</v>
@@ -6246,7 +6247,7 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
@@ -6270,7 +6271,7 @@
         <v>45</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6281,7 +6282,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6307,10 +6308,10 @@
         <v>57</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>366</v>
+      </c>
+      <c r="L40" t="s" s="2">
         <v>367</v>
-      </c>
-      <c r="L40" t="s" s="2">
-        <v>368</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -6361,7 +6362,7 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
@@ -6382,10 +6383,10 @@
         <v>45</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6396,7 +6397,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6419,16 +6420,16 @@
         <v>56</v>
       </c>
       <c r="J41" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="K41" t="s" s="2">
         <v>371</v>
       </c>
-      <c r="K41" t="s" s="2">
+      <c r="L41" t="s" s="2">
         <v>372</v>
       </c>
-      <c r="L41" t="s" s="2">
+      <c r="M41" t="s" s="2">
         <v>373</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>374</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
@@ -6478,7 +6479,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6499,10 +6500,10 @@
         <v>45</v>
       </c>
       <c r="AL41" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="AM41" t="s" s="2">
         <v>375</v>
-      </c>
-      <c r="AM41" t="s" s="2">
-        <v>376</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
@@ -6513,7 +6514,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6536,16 +6537,16 @@
         <v>56</v>
       </c>
       <c r="J42" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="K42" t="s" s="2">
         <v>378</v>
       </c>
-      <c r="K42" t="s" s="2">
+      <c r="L42" t="s" s="2">
         <v>379</v>
       </c>
-      <c r="L42" t="s" s="2">
+      <c r="M42" t="s" s="2">
         <v>380</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>381</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
@@ -6595,7 +6596,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6616,10 +6617,10 @@
         <v>45</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6630,7 +6631,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6653,19 +6654,19 @@
         <v>56</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="L43" t="s" s="2">
         <v>384</v>
       </c>
-      <c r="L43" t="s" s="2">
+      <c r="M43" t="s" s="2">
         <v>385</v>
       </c>
-      <c r="M43" t="s" s="2">
+      <c r="N43" t="s" s="2">
         <v>386</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>387</v>
       </c>
       <c r="O43" t="s" s="2">
         <v>45</v>
@@ -6702,19 +6703,19 @@
         <v>45</v>
       </c>
       <c r="AA43" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="AB43" t="s" s="2">
         <v>388</v>
       </c>
-      <c r="AB43" t="s" s="2">
+      <c r="AC43" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD43" t="s" s="2">
         <v>389</v>
       </c>
-      <c r="AC43" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD43" t="s" s="2">
-        <v>390</v>
-      </c>
       <c r="AE43" t="s" s="2">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -6735,10 +6736,10 @@
         <v>45</v>
       </c>
       <c r="AL43" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="AM43" t="s" s="2">
         <v>391</v>
-      </c>
-      <c r="AM43" t="s" s="2">
-        <v>392</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
@@ -6749,7 +6750,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6775,10 +6776,10 @@
         <v>57</v>
       </c>
       <c r="K44" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="L44" t="s" s="2">
         <v>321</v>
-      </c>
-      <c r="L44" t="s" s="2">
-        <v>322</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -6829,7 +6830,7 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
@@ -6853,7 +6854,7 @@
         <v>45</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6864,7 +6865,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6893,7 +6894,7 @@
         <v>102</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="M45" t="s" s="2">
         <v>104</v>
@@ -6946,7 +6947,7 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
@@ -6970,7 +6971,7 @@
         <v>45</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6981,11 +6982,11 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
@@ -7007,10 +7008,10 @@
         <v>101</v>
       </c>
       <c r="K46" t="s" s="2">
+        <v>329</v>
+      </c>
+      <c r="L46" t="s" s="2">
         <v>330</v>
-      </c>
-      <c r="L46" t="s" s="2">
-        <v>331</v>
       </c>
       <c r="M46" t="s" s="2">
         <v>104</v>
@@ -7065,7 +7066,7 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -7100,7 +7101,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -7126,13 +7127,13 @@
         <v>153</v>
       </c>
       <c r="K47" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="L47" t="s" s="2">
         <v>397</v>
       </c>
-      <c r="L47" t="s" s="2">
+      <c r="M47" t="s" s="2">
         <v>398</v>
-      </c>
-      <c r="M47" t="s" s="2">
-        <v>399</v>
       </c>
       <c r="N47" t="s" s="2">
         <v>168</v>
@@ -7160,14 +7161,14 @@
         <v>45</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="X47" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="Y47" t="s" s="2">
         <v>400</v>
       </c>
-      <c r="Y47" t="s" s="2">
-        <v>401</v>
-      </c>
       <c r="Z47" t="s" s="2">
         <v>45</v>
       </c>
@@ -7184,7 +7185,7 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>55</v>
@@ -7202,7 +7203,7 @@
         <v>45</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AL47" t="s" s="2">
         <v>172</v>
@@ -7219,7 +7220,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7245,13 +7246,13 @@
         <v>232</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="L48" t="s" s="2">
         <v>234</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="N48" t="s" s="2">
         <v>236</v>
@@ -7303,7 +7304,7 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
@@ -7321,7 +7322,7 @@
         <v>45</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>240</v>
@@ -7338,7 +7339,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7364,13 +7365,13 @@
         <v>153</v>
       </c>
       <c r="K49" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="L49" t="s" s="2">
         <v>408</v>
       </c>
-      <c r="L49" t="s" s="2">
+      <c r="M49" t="s" s="2">
         <v>409</v>
-      </c>
-      <c r="M49" t="s" s="2">
-        <v>410</v>
       </c>
       <c r="N49" t="s" s="2">
         <v>247</v>
@@ -7422,7 +7423,7 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
@@ -7457,7 +7458,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7520,10 +7521,10 @@
         <v>248</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>259</v>
+        <v>411</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>260</v>
+        <v>412</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>45</v>
@@ -7541,7 +7542,7 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
@@ -7559,24 +7560,24 @@
         <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="AL50" t="s" s="2">
         <v>261</v>
       </c>
-      <c r="AL50" t="s" s="2">
+      <c r="AM50" t="s" s="2">
         <v>262</v>
       </c>
-      <c r="AM50" t="s" s="2">
+      <c r="AN50" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO50" t="s" s="2">
         <v>263</v>
-      </c>
-      <c r="AN50" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO50" t="s" s="2">
-        <v>264</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7602,16 +7603,16 @@
         <v>45</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="M51" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="N51" t="s" s="2">
         <v>315</v>
-      </c>
-      <c r="N51" t="s" s="2">
-        <v>316</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7660,7 +7661,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7681,10 +7682,10 @@
         <v>45</v>
       </c>
       <c r="AL51" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="AM51" t="s" s="2">
         <v>318</v>
-      </c>
-      <c r="AM51" t="s" s="2">
-        <v>319</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>
@@ -7695,10 +7696,10 @@
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C52" t="s" s="2">
         <v>45</v>
@@ -7720,19 +7721,19 @@
         <v>56</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K52" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="L52" t="s" s="2">
         <v>384</v>
       </c>
-      <c r="L52" t="s" s="2">
+      <c r="M52" t="s" s="2">
         <v>385</v>
       </c>
-      <c r="M52" t="s" s="2">
+      <c r="N52" t="s" s="2">
         <v>386</v>
-      </c>
-      <c r="N52" t="s" s="2">
-        <v>387</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>45</v>
@@ -7781,7 +7782,7 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
@@ -7802,10 +7803,10 @@
         <v>45</v>
       </c>
       <c r="AL52" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="AM52" t="s" s="2">
         <v>391</v>
-      </c>
-      <c r="AM52" t="s" s="2">
-        <v>392</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>45</v>
@@ -7816,7 +7817,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7842,10 +7843,10 @@
         <v>57</v>
       </c>
       <c r="K53" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="L53" t="s" s="2">
         <v>321</v>
-      </c>
-      <c r="L53" t="s" s="2">
-        <v>322</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -7896,7 +7897,7 @@
         <v>45</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>43</v>
@@ -7920,7 +7921,7 @@
         <v>45</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>45</v>
@@ -7931,7 +7932,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7960,7 +7961,7 @@
         <v>102</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="M54" t="s" s="2">
         <v>104</v>
@@ -8013,7 +8014,7 @@
         <v>45</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>43</v>
@@ -8037,7 +8038,7 @@
         <v>45</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AN54" t="s" s="2">
         <v>45</v>
@@ -8048,11 +8049,11 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
@@ -8074,10 +8075,10 @@
         <v>101</v>
       </c>
       <c r="K55" t="s" s="2">
+        <v>329</v>
+      </c>
+      <c r="L55" t="s" s="2">
         <v>330</v>
-      </c>
-      <c r="L55" t="s" s="2">
-        <v>331</v>
       </c>
       <c r="M55" t="s" s="2">
         <v>104</v>
@@ -8132,7 +8133,7 @@
         <v>45</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>43</v>
@@ -8167,7 +8168,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -8193,13 +8194,13 @@
         <v>153</v>
       </c>
       <c r="K56" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="L56" t="s" s="2">
         <v>397</v>
       </c>
-      <c r="L56" t="s" s="2">
+      <c r="M56" t="s" s="2">
         <v>398</v>
-      </c>
-      <c r="M56" t="s" s="2">
-        <v>399</v>
       </c>
       <c r="N56" t="s" s="2">
         <v>168</v>
@@ -8212,7 +8213,7 @@
         <v>45</v>
       </c>
       <c r="R56" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="S56" t="s" s="2">
         <v>45</v>
@@ -8227,14 +8228,14 @@
         <v>45</v>
       </c>
       <c r="W56" t="s" s="2">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="X56" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="Y56" t="s" s="2">
         <v>400</v>
       </c>
-      <c r="Y56" t="s" s="2">
-        <v>401</v>
-      </c>
       <c r="Z56" t="s" s="2">
         <v>45</v>
       </c>
@@ -8251,7 +8252,7 @@
         <v>45</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>55</v>
@@ -8269,7 +8270,7 @@
         <v>45</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>172</v>
@@ -8286,7 +8287,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -8309,16 +8310,16 @@
         <v>56</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="L57" t="s" s="2">
         <v>234</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="N57" t="s" s="2">
         <v>236</v>
@@ -8358,17 +8359,17 @@
         <v>45</v>
       </c>
       <c r="AA57" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="AB57" s="2"/>
       <c r="AC57" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD57" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>43</v>
@@ -8386,7 +8387,7 @@
         <v>45</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="AL57" t="s" s="2">
         <v>240</v>
@@ -8403,10 +8404,10 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C58" t="s" s="2">
         <v>45</v>
@@ -8428,16 +8429,16 @@
         <v>56</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="L58" t="s" s="2">
         <v>234</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="N58" t="s" s="2">
         <v>236</v>
@@ -8489,7 +8490,7 @@
         <v>45</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>43</v>
@@ -8507,7 +8508,7 @@
         <v>45</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>240</v>
@@ -8524,7 +8525,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -8550,10 +8551,10 @@
         <v>57</v>
       </c>
       <c r="K59" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="L59" t="s" s="2">
         <v>321</v>
-      </c>
-      <c r="L59" t="s" s="2">
-        <v>322</v>
       </c>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -8604,7 +8605,7 @@
         <v>45</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>43</v>
@@ -8628,7 +8629,7 @@
         <v>45</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AN59" t="s" s="2">
         <v>45</v>
@@ -8639,7 +8640,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8668,7 +8669,7 @@
         <v>102</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="M60" t="s" s="2">
         <v>104</v>
@@ -8709,19 +8710,19 @@
         <v>45</v>
       </c>
       <c r="AA60" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AB60" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="AC60" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD60" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>43</v>
@@ -8745,7 +8746,7 @@
         <v>45</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AN60" t="s" s="2">
         <v>45</v>
@@ -8756,7 +8757,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8779,19 +8780,19 @@
         <v>56</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="N61" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>45</v>
@@ -8840,7 +8841,7 @@
         <v>45</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>43</v>
@@ -8861,10 +8862,10 @@
         <v>45</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AM61" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="AN61" t="s" s="2">
         <v>45</v>
@@ -8875,7 +8876,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8901,20 +8902,20 @@
         <v>75</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="M62" s="2"/>
       <c r="N62" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="O62" t="s" s="2">
         <v>45</v>
       </c>
       <c r="P62" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="Q62" t="s" s="2">
         <v>45</v>
@@ -8938,10 +8939,10 @@
         <v>144</v>
       </c>
       <c r="X62" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="Y62" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="Z62" t="s" s="2">
         <v>45</v>
@@ -8959,7 +8960,7 @@
         <v>45</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>43</v>
@@ -8980,10 +8981,10 @@
         <v>45</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="AM62" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="AN62" t="s" s="2">
         <v>45</v>
@@ -8994,7 +8995,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -9020,14 +9021,14 @@
         <v>57</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="M63" s="2"/>
       <c r="N63" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="O63" t="s" s="2">
         <v>45</v>
@@ -9037,7 +9038,7 @@
         <v>45</v>
       </c>
       <c r="R63" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="S63" t="s" s="2">
         <v>45</v>
@@ -9076,7 +9077,7 @@
         <v>45</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>43</v>
@@ -9097,10 +9098,10 @@
         <v>45</v>
       </c>
       <c r="AL63" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AM63" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AN63" t="s" s="2">
         <v>45</v>
@@ -9111,7 +9112,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -9137,14 +9138,14 @@
         <v>69</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="M64" s="2"/>
       <c r="N64" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="O64" t="s" s="2">
         <v>45</v>
@@ -9154,7 +9155,7 @@
         <v>45</v>
       </c>
       <c r="R64" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="S64" t="s" s="2">
         <v>45</v>
@@ -9193,7 +9194,7 @@
         <v>45</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>43</v>
@@ -9202,7 +9203,7 @@
         <v>55</v>
       </c>
       <c r="AH64" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="AI64" t="s" s="2">
         <v>67</v>
@@ -9214,10 +9215,10 @@
         <v>45</v>
       </c>
       <c r="AL64" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AM64" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="AN64" t="s" s="2">
         <v>45</v>
@@ -9228,7 +9229,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -9254,16 +9255,16 @@
         <v>75</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="N65" t="s" s="2">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="O65" t="s" s="2">
         <v>45</v>
@@ -9273,7 +9274,7 @@
         <v>45</v>
       </c>
       <c r="R65" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="S65" t="s" s="2">
         <v>45</v>
@@ -9312,7 +9313,7 @@
         <v>45</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>43</v>
@@ -9333,10 +9334,10 @@
         <v>45</v>
       </c>
       <c r="AL65" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AM65" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="AN65" t="s" s="2">
         <v>45</v>
@@ -9347,7 +9348,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -9373,13 +9374,13 @@
         <v>153</v>
       </c>
       <c r="K66" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="L66" t="s" s="2">
         <v>408</v>
       </c>
-      <c r="L66" t="s" s="2">
+      <c r="M66" t="s" s="2">
         <v>409</v>
-      </c>
-      <c r="M66" t="s" s="2">
-        <v>410</v>
       </c>
       <c r="N66" t="s" s="2">
         <v>247</v>
@@ -9431,7 +9432,7 @@
         <v>45</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>43</v>
@@ -9466,7 +9467,7 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -9529,10 +9530,10 @@
         <v>248</v>
       </c>
       <c r="X67" t="s" s="2">
-        <v>259</v>
+        <v>411</v>
       </c>
       <c r="Y67" t="s" s="2">
-        <v>260</v>
+        <v>412</v>
       </c>
       <c r="Z67" t="s" s="2">
         <v>45</v>
@@ -9550,7 +9551,7 @@
         <v>45</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>43</v>
@@ -9568,24 +9569,24 @@
         <v>45</v>
       </c>
       <c r="AK67" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="AL67" t="s" s="2">
         <v>261</v>
       </c>
-      <c r="AL67" t="s" s="2">
+      <c r="AM67" t="s" s="2">
         <v>262</v>
       </c>
-      <c r="AM67" t="s" s="2">
+      <c r="AN67" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO67" t="s" s="2">
         <v>263</v>
-      </c>
-      <c r="AN67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO67" t="s" s="2">
-        <v>264</v>
       </c>
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -9611,16 +9612,16 @@
         <v>45</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="M68" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="N68" t="s" s="2">
         <v>315</v>
-      </c>
-      <c r="N68" t="s" s="2">
-        <v>316</v>
       </c>
       <c r="O68" t="s" s="2">
         <v>45</v>
@@ -9669,7 +9670,7 @@
         <v>45</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>43</v>
@@ -9690,10 +9691,10 @@
         <v>45</v>
       </c>
       <c r="AL68" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="AM68" t="s" s="2">
         <v>318</v>
-      </c>
-      <c r="AM68" t="s" s="2">
-        <v>319</v>
       </c>
       <c r="AN68" t="s" s="2">
         <v>45</v>

</xml_diff>